<commit_message>
update w/ more fixtures
</commit_message>
<xml_diff>
--- a/Shows/Musical/Patch Plan.xlsx
+++ b/Shows/Musical/Patch Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub Onyx\Onyx-Tutorial\Shows\Musical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED288A87-13DF-4645-885F-183C4F45AE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF9DA68-2F3B-422F-BF61-3DEDFD707DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5925" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30375" yWindow="-4740" windowWidth="13695" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="112">
   <si>
     <t>Type</t>
   </si>
@@ -280,6 +280,87 @@
   </si>
   <si>
     <t>--</t>
+  </si>
+  <si>
+    <t>Clay Paky</t>
+  </si>
+  <si>
+    <t>Alpha Beam 700</t>
+  </si>
+  <si>
+    <t>B.184</t>
+  </si>
+  <si>
+    <t>B.206</t>
+  </si>
+  <si>
+    <t>B.228</t>
+  </si>
+  <si>
+    <t>B.250</t>
+  </si>
+  <si>
+    <t>B.272</t>
+  </si>
+  <si>
+    <t>B.294</t>
+  </si>
+  <si>
+    <t>B.316</t>
+  </si>
+  <si>
+    <t>B.338</t>
+  </si>
+  <si>
+    <t>B.360</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standart </t>
+  </si>
+  <si>
+    <t>Left Truss 1</t>
+  </si>
+  <si>
+    <t>Left Truss 2</t>
+  </si>
+  <si>
+    <t>Left Truss 3</t>
+  </si>
+  <si>
+    <t>B.382</t>
+  </si>
+  <si>
+    <t>B.404</t>
+  </si>
+  <si>
+    <t>B.426</t>
+  </si>
+  <si>
+    <t>Right Truss 3</t>
+  </si>
+  <si>
+    <t>C.001</t>
+  </si>
+  <si>
+    <t>C.023</t>
+  </si>
+  <si>
+    <t>C.045</t>
+  </si>
+  <si>
+    <t>C.067</t>
+  </si>
+  <si>
+    <t>C.089</t>
+  </si>
+  <si>
+    <t>C.111</t>
+  </si>
+  <si>
+    <t>Right Truss 2</t>
+  </si>
+  <si>
+    <t>Right Truss 1</t>
   </si>
 </sst>
 </file>
@@ -307,7 +388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +467,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -399,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -419,6 +512,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -708,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1641,6 +1736,278 @@
         <v>40</v>
       </c>
     </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>